<commit_message>
finalized contentsMap, locationsMap, dependenceMap and their usages. Designed and coded the update of dependants in case their decisive fields change, many other changes, enabled DB Connection for dependences etc...
</commit_message>
<xml_diff>
--- a/implicaspection/report-templates/a2yorumkod-Bericht2_MitKommentaren2.xlsx
+++ b/implicaspection/report-templates/a2yorumkod-Bericht2_MitKommentaren2.xlsx
@@ -113,8 +113,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">???combo???Müşteri Adı???musteri-adi
-</t>
+          <t xml:space="preserve">???combo???Müşteri Adı???musteri-adi</t>
         </r>
       </text>
     </comment>
@@ -1243,7 +1242,7 @@
             <family val="2"/>
             <charset val="162"/>
           </rPr>
-          <t xml:space="preserve">???rapor-no???Rapor No</t>
+          <t xml:space="preserve">???special???Rapor No???rapor-no</t>
         </r>
       </text>
     </comment>
@@ -1257,7 +1256,7 @@
             <family val="2"/>
             <charset val="162"/>
           </rPr>
-          <t xml:space="preserve">???rapor-tarihi???Rapor Tarihi</t>
+          <t xml:space="preserve">???special???Rapor Tarihi???rapor-tarihi</t>
         </r>
       </text>
     </comment>
@@ -3661,7 +3660,7 @@
   <dimension ref="A1:AO74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T3" activeCellId="0" sqref="T3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
improved logging, added error logging, started working on specially requested fields such as rapor-no
</commit_message>
<xml_diff>
--- a/implicaspection/report-templates/a2yorumkod-Bericht2_MitKommentaren2.xlsx
+++ b/implicaspection/report-templates/a2yorumkod-Bericht2_MitKommentaren2.xlsx
@@ -112,6 +112,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">???combo???Müşteri Adı???musteri-adi</t>
         </r>
@@ -3017,6 +3018,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -3584,9 +3586,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>13680</xdr:colOff>
+      <xdr:colOff>13320</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>197640</xdr:rowOff>
+      <xdr:rowOff>197280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3600,7 +3602,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2276280" y="5213880"/>
-          <a:ext cx="1520640" cy="1078920"/>
+          <a:ext cx="1520280" cy="1078560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3621,9 +3623,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>149760</xdr:colOff>
+      <xdr:colOff>149400</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3637,7 +3639,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="74160" y="5230080"/>
-          <a:ext cx="1781640" cy="901080"/>
+          <a:ext cx="1781280" cy="900720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3660,7 +3662,7 @@
   <dimension ref="A1:AO74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Can now change the default values of default-valued-fields. Some other major fixes
</commit_message>
<xml_diff>
--- a/implicaspection/report-templates/a2yorumkod-Bericht2_MitKommentaren2.xlsx
+++ b/implicaspection/report-templates/a2yorumkod-Bericht2_MitKommentaren2.xlsx
@@ -148,16 +148,7 @@
     </comment>
     <comment ref="D6" authorId="0">
       <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="162"/>
-          </rPr>
-          <t xml:space="preserve">???default???Muayene Standardı???muayene-standardi???TS EN ISO 17638</t>
-        </r>
+        <t>???default???Muayene Standardı???muayene-standardi???TS EN ISO 17622</t>
       </text>
     </comment>
     <comment ref="D7" authorId="0">
@@ -892,17 +883,7 @@
     </comment>
     <comment ref="T5" authorId="0">
       <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="162"/>
-          </rPr>
-          <t xml:space="preserve">???default???Resim No???resim-no???-</t>
-        </r>
+        <t>???default???Resim No???resim-no???-55f</t>
       </text>
     </comment>
     <comment ref="T6" authorId="0">
@@ -1320,10 +1301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="115">
-  <si>
-    <t xml:space="preserve">şablondur</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="114">
   <si>
     <t xml:space="preserve"> GÖZETİM MUAYENE VE EĞİTİM HİZMETLERİ</t>
   </si>
@@ -3586,9 +3564,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>13320</xdr:colOff>
+      <xdr:colOff>12960</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>197280</xdr:rowOff>
+      <xdr:rowOff>196920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3602,7 +3580,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2276280" y="5213880"/>
-          <a:ext cx="1520280" cy="1078560"/>
+          <a:ext cx="1519920" cy="1078200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3623,9 +3601,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>149400</xdr:colOff>
+      <xdr:colOff>149040</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>35640</xdr:rowOff>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3639,7 +3617,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="74160" y="5230080"/>
-          <a:ext cx="1781280" cy="900720"/>
+          <a:ext cx="1780920" cy="900360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3659,48 +3637,46 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AO74"/>
+  <dimension ref="A1:AO429"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="AE23" activeCellId="0" sqref="AE23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="0.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="4.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="0.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="3.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="5.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="3.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="4.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="1" width="0.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="4.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="3.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="3.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="0.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="2.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="5.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="4.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="6.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="29" style="1" width="8.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="36" style="1" width="8.82"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="7.27" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="3" customWidth="true" hidden="false" style="1" width="5.28" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="0.82" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="4.71" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="0.82" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="4.17" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="1" width="3.27" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="5.55" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="3.45" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="1" width="5.72" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="4.82" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="15" customWidth="true" hidden="false" style="1" width="0.82" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="8.72" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="3.71" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="10.73" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="4.82" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="3.83" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="1" width="3.45" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="1" width="0.82" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="10.73" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="24" customWidth="true" hidden="false" style="1" width="2.46" collapsed="true" outlineLevel="0"/>
+    <col min="25" max="25" customWidth="true" hidden="false" style="1" width="5.72" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="4.71" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="6.72" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="7.82" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="34" customWidth="true" hidden="false" style="1" width="8.82" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="16.81" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="1025" customWidth="true" hidden="false" style="1" width="8.82" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -3708,7 +3684,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -3740,7 +3716,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -3765,12 +3741,12 @@
     </row>
     <row r="3" s="10" customFormat="true" ht="28.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -3785,18 +3761,18 @@
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="T3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
       <c r="X3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
@@ -3807,12 +3783,12 @@
     </row>
     <row r="4" s="10" customFormat="true" ht="28.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -3827,7 +3803,7 @@
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
@@ -3838,7 +3814,7 @@
       <c r="V4" s="14"/>
       <c r="W4" s="14"/>
       <c r="X4" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y4" s="13"/>
       <c r="Z4" s="13"/>
@@ -3847,25 +3823,25 @@
       </c>
       <c r="AB4" s="15"/>
       <c r="AF4" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AG4" s="10" t="n">
         <v>1</v>
       </c>
       <c r="AH4" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AI4" s="10" t="n">
         <v>2</v>
       </c>
       <c r="AJ4" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AK4" s="10" t="n">
         <v>3</v>
       </c>
       <c r="AN4" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AO4" s="10" t="n">
         <v>4</v>
@@ -3873,12 +3849,12 @@
     </row>
     <row r="5" s="10" customFormat="true" ht="28.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
@@ -3893,18 +3869,18 @@
       <c r="O5" s="16"/>
       <c r="P5" s="16"/>
       <c r="Q5" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R5" s="13"/>
       <c r="S5" s="13"/>
       <c r="T5" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U5" s="17"/>
       <c r="V5" s="17"/>
       <c r="W5" s="17"/>
       <c r="X5" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y5" s="13"/>
       <c r="Z5" s="13"/>
@@ -3913,26 +3889,26 @@
       </c>
       <c r="AB5" s="18"/>
       <c r="AG5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AI5" s="10" t="s">
+      <c r="AK5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="AK5" s="10" t="s">
+      <c r="AO5" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="AO5" s="10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" s="10" customFormat="true" ht="28.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
@@ -3947,18 +3923,18 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R6" s="13"/>
       <c r="S6" s="13"/>
       <c r="T6" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U6" s="17"/>
       <c r="V6" s="17"/>
       <c r="W6" s="17"/>
       <c r="X6" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Y6" s="13"/>
       <c r="Z6" s="13"/>
@@ -3969,12 +3945,12 @@
     </row>
     <row r="7" s="10" customFormat="true" ht="28.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
       <c r="D7" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
@@ -3989,29 +3965,29 @@
       <c r="O7" s="20"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="21"/>
       <c r="T7" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U7" s="22"/>
       <c r="V7" s="22"/>
       <c r="W7" s="22"/>
       <c r="X7" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y7" s="21"/>
       <c r="Z7" s="21"/>
       <c r="AA7" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB7" s="23"/>
     </row>
     <row r="8" s="10" customFormat="true" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
@@ -4043,13 +4019,13 @@
     </row>
     <row r="9" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
@@ -4057,7 +4033,7 @@
       <c r="I9" s="25"/>
       <c r="J9" s="25"/>
       <c r="K9" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
@@ -4065,7 +4041,7 @@
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R9" s="25"/>
       <c r="S9" s="25"/>
@@ -4073,28 +4049,28 @@
       <c r="U9" s="25"/>
       <c r="V9" s="25"/>
       <c r="W9" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X9" s="13"/>
       <c r="Y9" s="13"/>
       <c r="Z9" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA9" s="26"/>
       <c r="AB9" s="26"/>
       <c r="AF9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
@@ -4102,7 +4078,7 @@
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
       <c r="K10" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
@@ -4110,7 +4086,7 @@
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
@@ -4118,28 +4094,28 @@
       <c r="U10" s="25"/>
       <c r="V10" s="25"/>
       <c r="W10" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="X10" s="27"/>
       <c r="Y10" s="27"/>
       <c r="Z10" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AA10" s="26"/>
       <c r="AB10" s="26"/>
       <c r="AF10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
@@ -4147,7 +4123,7 @@
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
       <c r="K11" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
@@ -4155,7 +4131,7 @@
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
@@ -4171,7 +4147,7 @@
     </row>
     <row r="12" s="30" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -4183,7 +4159,7 @@
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
       <c r="K12" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
@@ -4197,25 +4173,25 @@
       <c r="U12" s="28"/>
       <c r="V12" s="28"/>
       <c r="W12" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
       <c r="Z12" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AA12" s="29"/>
       <c r="AB12" s="29"/>
     </row>
     <row r="13" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
@@ -4223,7 +4199,7 @@
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>
       <c r="K13" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
@@ -4237,25 +4213,25 @@
       <c r="U13" s="25"/>
       <c r="V13" s="25"/>
       <c r="W13" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X13" s="27"/>
       <c r="Y13" s="27"/>
       <c r="Z13" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA13" s="26"/>
       <c r="AB13" s="26"/>
     </row>
     <row r="14" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14" s="31"/>
       <c r="G14" s="31"/>
@@ -4263,7 +4239,7 @@
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
       <c r="K14" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
@@ -4277,17 +4253,17 @@
       <c r="U14" s="32"/>
       <c r="V14" s="32"/>
       <c r="W14" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X14" s="33"/>
       <c r="Y14" s="33"/>
       <c r="Z14" s="34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AA14" s="34"/>
       <c r="AB14" s="34"/>
       <c r="AF14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4299,7 +4275,7 @@
       <c r="F15" s="35"/>
       <c r="G15" s="35"/>
       <c r="H15" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I15" s="36"/>
       <c r="J15" s="36"/>
@@ -4310,7 +4286,7 @@
       <c r="O15" s="36"/>
       <c r="P15" s="36"/>
       <c r="Q15" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R15" s="37"/>
       <c r="S15" s="37"/>
@@ -4342,11 +4318,11 @@
       <c r="O16" s="36"/>
       <c r="P16" s="36"/>
       <c r="Q16" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R16" s="38"/>
       <c r="S16" s="39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T16" s="39"/>
       <c r="U16" s="39"/>
@@ -4376,11 +4352,11 @@
       <c r="O17" s="36"/>
       <c r="P17" s="36"/>
       <c r="Q17" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R17" s="40"/>
       <c r="S17" s="41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T17" s="41"/>
       <c r="U17" s="41"/>
@@ -4410,11 +4386,11 @@
       <c r="O18" s="36"/>
       <c r="P18" s="36"/>
       <c r="Q18" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R18" s="40"/>
       <c r="S18" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T18" s="39"/>
       <c r="U18" s="39"/>
@@ -4444,11 +4420,11 @@
       <c r="O19" s="36"/>
       <c r="P19" s="36"/>
       <c r="Q19" s="42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R19" s="42"/>
       <c r="S19" s="43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T19" s="43"/>
       <c r="U19" s="43"/>
@@ -4462,7 +4438,7 @@
     </row>
     <row r="20" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
@@ -4471,7 +4447,7 @@
       <c r="F20" s="44"/>
       <c r="G20" s="44"/>
       <c r="H20" s="45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I20" s="45"/>
       <c r="J20" s="45"/>
@@ -4496,7 +4472,7 @@
     </row>
     <row r="21" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="46"/>
       <c r="C21" s="46"/>
@@ -4530,7 +4506,7 @@
     </row>
     <row r="22" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
@@ -4562,7 +4538,7 @@
     </row>
     <row r="23" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" s="50"/>
       <c r="C23" s="50"/>
@@ -4594,10 +4570,10 @@
     </row>
     <row r="24" s="10" customFormat="true" ht="28.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="27" t="s">
         <v>82</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>83</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
@@ -4606,12 +4582,12 @@
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
       <c r="I24" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J24" s="27"/>
       <c r="K24" s="27"/>
       <c r="L24" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M24" s="27"/>
       <c r="N24" s="27"/>
@@ -4619,25 +4595,25 @@
       <c r="P24" s="27"/>
       <c r="Q24" s="27"/>
       <c r="R24" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="S24" s="27" t="s">
         <v>86</v>
-      </c>
-      <c r="S24" s="27" t="s">
-        <v>87</v>
       </c>
       <c r="T24" s="27"/>
       <c r="U24" s="27"/>
       <c r="V24" s="27"/>
       <c r="W24" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="X24" s="27"/>
       <c r="Y24" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Z24" s="27"/>
       <c r="AA24" s="27"/>
       <c r="AB24" s="52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4645,7 +4621,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="54"/>
       <c r="D25" s="54"/>
@@ -4659,7 +4635,7 @@
       <c r="J25" s="55"/>
       <c r="K25" s="55"/>
       <c r="L25" s="55" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M25" s="55"/>
       <c r="N25" s="55"/>
@@ -4670,7 +4646,7 @@
         <v>12</v>
       </c>
       <c r="S25" s="56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="T25" s="56"/>
       <c r="U25" s="56"/>
@@ -4681,7 +4657,7 @@
       <c r="Z25" s="55"/>
       <c r="AA25" s="55"/>
       <c r="AB25" s="57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4689,7 +4665,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" s="54"/>
       <c r="D26" s="54"/>
@@ -4703,7 +4679,7 @@
       <c r="J26" s="55"/>
       <c r="K26" s="55"/>
       <c r="L26" s="55" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M26" s="55"/>
       <c r="N26" s="55"/>
@@ -4714,7 +4690,7 @@
         <v>12</v>
       </c>
       <c r="S26" s="56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="T26" s="56"/>
       <c r="U26" s="56"/>
@@ -4725,7 +4701,7 @@
       <c r="Z26" s="55"/>
       <c r="AA26" s="55"/>
       <c r="AB26" s="57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4733,7 +4709,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" s="54"/>
       <c r="D27" s="54"/>
@@ -4747,7 +4723,7 @@
       <c r="J27" s="55"/>
       <c r="K27" s="55"/>
       <c r="L27" s="55" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M27" s="55"/>
       <c r="N27" s="55"/>
@@ -4758,7 +4734,7 @@
         <v>12</v>
       </c>
       <c r="S27" s="56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="T27" s="56"/>
       <c r="U27" s="56"/>
@@ -4769,7 +4745,7 @@
       <c r="Z27" s="55"/>
       <c r="AA27" s="55"/>
       <c r="AB27" s="57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4777,7 +4753,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C28" s="54"/>
       <c r="D28" s="54"/>
@@ -4791,7 +4767,7 @@
       <c r="J28" s="55"/>
       <c r="K28" s="55"/>
       <c r="L28" s="55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M28" s="55"/>
       <c r="N28" s="55"/>
@@ -4802,7 +4778,7 @@
         <v>12</v>
       </c>
       <c r="S28" s="56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="T28" s="56"/>
       <c r="U28" s="56"/>
@@ -4813,7 +4789,7 @@
       <c r="Z28" s="55"/>
       <c r="AA28" s="55"/>
       <c r="AB28" s="57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4821,7 +4797,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29" s="54"/>
       <c r="D29" s="54"/>
@@ -4835,7 +4811,7 @@
       <c r="J29" s="55"/>
       <c r="K29" s="55"/>
       <c r="L29" s="55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M29" s="55"/>
       <c r="N29" s="55"/>
@@ -4846,7 +4822,7 @@
         <v>12</v>
       </c>
       <c r="S29" s="56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="T29" s="56"/>
       <c r="U29" s="56"/>
@@ -4857,7 +4833,7 @@
       <c r="Z29" s="55"/>
       <c r="AA29" s="55"/>
       <c r="AB29" s="57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4865,7 +4841,7 @@
         <v>6</v>
       </c>
       <c r="B30" s="54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C30" s="54"/>
       <c r="D30" s="54"/>
@@ -4879,7 +4855,7 @@
       <c r="J30" s="55"/>
       <c r="K30" s="55"/>
       <c r="L30" s="55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M30" s="55"/>
       <c r="N30" s="55"/>
@@ -4890,7 +4866,7 @@
         <v>12</v>
       </c>
       <c r="S30" s="56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="T30" s="56"/>
       <c r="U30" s="56"/>
@@ -4901,7 +4877,7 @@
       <c r="Z30" s="55"/>
       <c r="AA30" s="55"/>
       <c r="AB30" s="57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4909,7 +4885,7 @@
         <v>7</v>
       </c>
       <c r="B31" s="54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="54"/>
       <c r="D31" s="54"/>
@@ -4923,7 +4899,7 @@
       <c r="J31" s="55"/>
       <c r="K31" s="55"/>
       <c r="L31" s="55" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M31" s="55"/>
       <c r="N31" s="55"/>
@@ -4934,7 +4910,7 @@
         <v>4</v>
       </c>
       <c r="S31" s="56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T31" s="56"/>
       <c r="U31" s="56"/>
@@ -4945,7 +4921,7 @@
       <c r="Z31" s="55"/>
       <c r="AA31" s="55"/>
       <c r="AB31" s="57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5174,14 +5150,14 @@
     </row>
     <row r="39" s="10" customFormat="true" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B39" s="44"/>
       <c r="C39" s="44"/>
       <c r="D39" s="44"/>
       <c r="E39" s="44"/>
       <c r="F39" s="63" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G39" s="63"/>
       <c r="H39" s="63"/>
@@ -5193,35 +5169,35 @@
       <c r="N39" s="63"/>
       <c r="O39" s="63"/>
       <c r="P39" s="63" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q39" s="63"/>
       <c r="R39" s="63"/>
       <c r="S39" s="63"/>
       <c r="T39" s="63"/>
       <c r="U39" s="63" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="V39" s="63"/>
       <c r="W39" s="63"/>
       <c r="X39" s="63"/>
       <c r="Y39" s="63"/>
       <c r="Z39" s="64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA39" s="64"/>
       <c r="AB39" s="64"/>
     </row>
     <row r="40" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="65" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B40" s="65"/>
       <c r="C40" s="65"/>
       <c r="D40" s="65"/>
       <c r="E40" s="65"/>
       <c r="F40" s="66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G40" s="66"/>
       <c r="H40" s="66"/>
@@ -5233,14 +5209,14 @@
       <c r="N40" s="66"/>
       <c r="O40" s="66"/>
       <c r="P40" s="66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q40" s="66"/>
       <c r="R40" s="66"/>
       <c r="S40" s="66"/>
       <c r="T40" s="66"/>
       <c r="U40" s="66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V40" s="66"/>
       <c r="W40" s="66"/>
@@ -5252,14 +5228,14 @@
     </row>
     <row r="41" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B41" s="65"/>
       <c r="C41" s="65"/>
       <c r="D41" s="65"/>
       <c r="E41" s="65"/>
       <c r="F41" s="68" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G41" s="68"/>
       <c r="H41" s="68"/>
@@ -5271,14 +5247,14 @@
       <c r="N41" s="68"/>
       <c r="O41" s="68"/>
       <c r="P41" s="68" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q41" s="68"/>
       <c r="R41" s="68"/>
       <c r="S41" s="68"/>
       <c r="T41" s="68"/>
       <c r="U41" s="66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V41" s="66"/>
       <c r="W41" s="66"/>
@@ -5290,7 +5266,7 @@
     </row>
     <row r="42" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="65" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B42" s="65"/>
       <c r="C42" s="65"/>
@@ -5328,7 +5304,7 @@
     </row>
     <row r="43" customFormat="false" ht="57.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="71" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B43" s="71"/>
       <c r="C43" s="71"/>
@@ -5360,7 +5336,7 @@
     </row>
     <row r="44" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="74" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B44" s="74"/>
       <c r="C44" s="74"/>

</xml_diff>

<commit_message>
many major changes, removal of combobox values etc
</commit_message>
<xml_diff>
--- a/implicaspection/report-templates/a2yorumkod-Bericht2_MitKommentaren2.xlsx
+++ b/implicaspection/report-templates/a2yorumkod-Bericht2_MitKommentaren2.xlsx
@@ -148,7 +148,7 @@
     </comment>
     <comment ref="D6" authorId="0">
       <text>
-        <t>???default???Muayene Standardı???muayene-standardi???TS EN ISO 17622</t>
+        <t>???default???Muayene Standardı???muayene-standardi???TS EN ISO 17638</t>
       </text>
     </comment>
     <comment ref="D7" authorId="0">
@@ -855,16 +855,7 @@
     </comment>
     <comment ref="T3" authorId="0">
       <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="162"/>
-          </rPr>
-          <t xml:space="preserve">???default???Muayene Prosedürü???muayene-proseduru???P-101-004</t>
-        </r>
+        <t>???default???Muayene Prosedürü???muayene-proseduru???P-101-004</t>
       </text>
     </comment>
     <comment ref="T4" authorId="0">
@@ -883,7 +874,7 @@
     </comment>
     <comment ref="T5" authorId="0">
       <text>
-        <t>???default???Resim No???resim-no???-55f</t>
+        <t>???default???Resim No???resim-no???-</t>
       </text>
     </comment>
     <comment ref="T6" authorId="0">
@@ -1202,16 +1193,7 @@
     </comment>
     <comment ref="AA3" authorId="0">
       <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="162"/>
-          </rPr>
-          <t xml:space="preserve">???default???Sayfa No???sayfa-no???1</t>
-        </r>
+        <t>???default???Sayfa No???sayfa-no???1</t>
       </text>
     </comment>
     <comment ref="AA4" authorId="0">

</xml_diff>